<commit_message>
excel files labeled by task
</commit_message>
<xml_diff>
--- a/BING690 HW & TESTS/Assigment 1 Rafael Villasmil BINF690 Fall 2020.xlsx
+++ b/BING690 HW & TESTS/Assigment 1 Rafael Villasmil BINF690 Fall 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parent/Documents/Professional Records/PhD GMU/BINF690 Numerical Methods in Bioinformatics Fall 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\villasmilr\Documents\GitHub\Assignments BINF690\BING690 HW &amp; TESTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42E1722-E5AC-2A49-8CF3-EAF3FBB44552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4662AC8C-F057-4CCD-A876-E6734E2A2868}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="460" windowWidth="31360" windowHeight="21940" xr2:uid="{A54DAB2A-24E1-A247-BB1A-78DA399D51EE}"/>
+    <workbookView xWindow="46680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{A54DAB2A-24E1-A247-BB1A-78DA399D51EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2026,34 +2035,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D46CC27-1F63-6243-B878-14FA58D6753E}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2075,7 +2084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2086,7 +2095,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2097,7 +2106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2116,7 +2125,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2124,12 +2133,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2137,7 +2146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f>B2</f>
         <v>0</v>
@@ -2190,7 +2199,7 @@
         <v>65.449846949787357</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>A14+$B$4</f>
         <v>0.25</v>
@@ -2220,7 +2229,7 @@
         <v>63.891583483285189</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ref="A16:A58" si="5">A15+$B$4</f>
         <v>0.5</v>
@@ -2250,7 +2259,7 @@
         <v>62.358251696081886</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="5"/>
         <v>0.75</v>
@@ -2280,7 +2289,7 @@
         <v>60.849650526247665</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="5"/>
         <v>1</v>
@@ -2310,7 +2319,7 @@
         <v>59.365578911852658</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="5"/>
         <v>1.25</v>
@@ -2340,7 +2349,7 @@
         <v>57.905835790967068</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="5"/>
         <v>1.5</v>
@@ -2370,7 +2379,7 @@
         <v>56.470220101661027</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="5"/>
         <v>1.75</v>
@@ -2400,7 +2409,7 @@
         <v>55.058530782004738</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="5"/>
         <v>2</v>
@@ -2430,7 +2439,7 @@
         <v>53.670566770068355</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="5"/>
         <v>2.25</v>
@@ -2460,7 +2469,7 @@
         <v>52.306127003922057</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="5"/>
         <v>2.5</v>
@@ -2490,7 +2499,7 @@
         <v>50.965010421636002</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="5"/>
         <v>2.75</v>
@@ -2520,7 +2529,7 @@
         <v>49.647015961280381</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -2550,7 +2559,7 @@
         <v>48.35194256092533</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="5"/>
         <v>3.25</v>
@@ -2580,7 +2589,7 @@
         <v>47.079589158641085</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="5"/>
         <v>3.5</v>
@@ -2610,7 +2619,7 @@
         <v>45.829754692497715</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="5"/>
         <v>3.75</v>
@@ -2640,7 +2649,7 @@
         <v>44.602238100565501</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -2670,7 +2679,7 @@
         <v>43.396838320914526</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="5"/>
         <v>4.25</v>
@@ -2700,7 +2709,7 @@
         <v>42.213354291614998</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="5"/>
         <v>4.5</v>
@@ -2730,7 +2739,7 @@
         <v>41.05158495073708</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="5"/>
         <v>4.75</v>
@@ -2760,7 +2769,7 @@
         <v>39.911329236350959</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="5"/>
         <v>5</v>
@@ -2790,7 +2799,7 @@
         <v>38.792386086526768</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="5"/>
         <v>5.25</v>
@@ -2820,7 +2829,7 @@
         <v>37.694554439334716</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>A35+$B$4</f>
         <v>5.5</v>
@@ -2850,7 +2859,7 @@
         <v>36.617633232844945</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="5"/>
         <v>5.75</v>
@@ -2880,7 +2889,7 @@
         <v>35.561421405127646</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="5"/>
         <v>6</v>
@@ -2910,7 +2919,7 @@
         <v>34.525717894252985</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="5"/>
         <v>6.25</v>
@@ -2940,7 +2949,7 @@
         <v>33.510321638291124</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="5"/>
         <v>6.5</v>
@@ -2970,7 +2979,7 @@
         <v>32.515031575312243</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="5"/>
         <v>6.75</v>
@@ -3000,7 +3009,7 @@
         <v>31.539646643386501</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="5"/>
         <v>7</v>
@@ -3030,7 +3039,7 @@
         <v>30.583965780584077</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="5"/>
         <v>7.25</v>
@@ -3060,7 +3069,7 @@
         <v>29.647787924975137</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="5"/>
         <v>7.5</v>
@@ -3090,7 +3099,7 @@
         <v>28.730912014629851</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="5"/>
         <v>7.75</v>
@@ -3120,7 +3129,7 @@
         <v>27.833136987618392</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="5"/>
         <v>8</v>
@@ -3150,7 +3159,7 @@
         <v>26.954261782010931</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="5"/>
         <v>8.25</v>
@@ -3180,7 +3189,7 @@
         <v>26.094085335877637</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="5"/>
         <v>8.5</v>
@@ -3210,7 +3219,7 @@
         <v>25.252406587288675</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="5"/>
         <v>8.75</v>
@@ -3240,7 +3249,7 @@
         <v>24.429024474314222</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="5"/>
         <v>9</v>
@@ -3270,7 +3279,7 @@
         <v>23.623737935024462</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="5"/>
         <v>9.25</v>
@@ -3300,7 +3309,7 @@
         <v>22.83634590748953</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="5"/>
         <v>9.5</v>
@@ -3330,7 +3339,7 @@
         <v>22.066647329779624</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="5"/>
         <v>9.75</v>
@@ -3360,7 +3369,7 @@
         <v>21.314441139964899</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <f t="shared" si="5"/>
         <v>10</v>
@@ -3390,7 +3399,7 @@
         <v>20.579526276115534</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="5"/>
         <v>10.25</v>
@@ -3420,7 +3429,7 @@
         <v>19.861701676301703</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="5"/>
         <v>10.5</v>
@@ -3450,7 +3459,7 @@
         <v>19.160766278593574</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="5"/>
         <v>10.75</v>
@@ -3480,7 +3489,7 @@
         <v>18.476519021061304</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="5"/>
         <v>11</v>

</xml_diff>